<commit_message>
V1 da Dissertação com o texto completo.
</commit_message>
<xml_diff>
--- a/ArtigoFormatoIEEE/R2R_SANER2015.xlsx
+++ b/ArtigoFormatoIEEE/R2R_SANER2015.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Revisão 1</t>
   </si>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +739,9 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
@@ -827,7 +829,9 @@
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
@@ -945,7 +949,9 @@
     </row>
     <row r="16" spans="1:5" ht="243" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="C16" s="6" t="s">
         <v>19</v>
       </c>
@@ -988,7 +994,9 @@
     </row>
     <row r="19" spans="1:5" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="C19" s="6" t="s">
         <v>21</v>
       </c>
@@ -1014,7 +1022,9 @@
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C21" s="6" t="s">
         <v>23</v>
       </c>
@@ -1027,7 +1037,9 @@
     </row>
     <row r="22" spans="1:5" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="C22" s="6" t="s">
         <v>24</v>
       </c>
@@ -1070,7 +1082,9 @@
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C25" s="6" t="s">
         <v>27</v>
       </c>
@@ -1083,7 +1097,9 @@
     </row>
     <row r="26" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="C26" s="6" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
V1 do artigo para o ASE 2015
</commit_message>
<xml_diff>
--- a/ArtigoFormatoIEEE/R2R_SANER2015.xlsx
+++ b/ArtigoFormatoIEEE/R2R_SANER2015.xlsx
@@ -15,10 +15,10 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$B$1:$D$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Plan1!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>Revisão 1</t>
   </si>
@@ -311,13 +311,7 @@
     <t>Reforce falando isso: que não há necessidade de instrumentação, e que esse repositório cópia é feito de forma transparente.</t>
   </si>
   <si>
-    <t>Artigo</t>
-  </si>
-  <si>
-    <t>Dissertação</t>
-  </si>
-  <si>
-    <t>OK</t>
+    <t>Item</t>
   </si>
 </sst>
 </file>
@@ -396,21 +390,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,418 +698,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.140625" customWidth="1"/>
-    <col min="5" max="5" width="55.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.140625" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>70</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="153" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="102.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="102.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="5" t="s">
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="153.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="243" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="3" t="s">
+    <row r="19" spans="1:4" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="243" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="6" t="s">
+    <row r="25" spans="1:4" s="1" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>21</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="6" t="s">
+      <c r="B25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
-  <conditionalFormatting sqref="A2:E26">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND($A2="OK",$B2="OK")</formula>
+  <autoFilter ref="B1:D1"/>
+  <conditionalFormatting sqref="B2:D26">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>AND(#REF!="OK",#REF!="OK")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>_xlfn.XOR($A2="OK",$B2="OK")</formula>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>_xlfn.XOR(#REF!="OK",#REF!="OK")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1126,7 +1083,7 @@
     <oddFooter>Página &amp;P de &amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="20" min="2" max="4" man="1"/>
+    <brk id="20" min="1" max="3" man="1"/>
   </rowBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>